<commit_message>
logs update and consolidation igarassu
</commit_message>
<xml_diff>
--- a/consolidacao/levantamento/2023_levantamento_CIGR.xlsx
+++ b/consolidacao/levantamento/2023_levantamento_CIGR.xlsx
@@ -7,14 +7,14 @@
     <sheet state="visible" name="Cópia de Respostas ao formulári" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Cópia de Respostas ao formulári'!$A$1:$Z$173</definedName>
+    <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'Cópia de Respostas ao formulári'!$A$1:$Z$180</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1860" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="484">
   <si>
     <t>Carimbo de data/hora</t>
   </si>
@@ -1391,6 +1391,60 @@
   </si>
   <si>
     <t>10.75</t>
+  </si>
+  <si>
+    <t>30.16.2119</t>
+  </si>
+  <si>
+    <t>Refil de tinta para marcador de quadro branco, modelo V Board Master, cor vermelha.</t>
+  </si>
+  <si>
+    <t>2.09</t>
+  </si>
+  <si>
+    <t>30.44.62</t>
+  </si>
+  <si>
+    <t>PLACA SETA INDICATIVA DE CO2.</t>
+  </si>
+  <si>
+    <t>9.8</t>
+  </si>
+  <si>
+    <t>30.44.61</t>
+  </si>
+  <si>
+    <t>PLACA SETA INDICATIVA DE AGUA PRESSURIZADA (AP).</t>
+  </si>
+  <si>
+    <t>21.89</t>
+  </si>
+  <si>
+    <t>30.22.143</t>
+  </si>
+  <si>
+    <t>SACO PLÁSTICO, 200 L, PCT C/ 100.</t>
+  </si>
+  <si>
+    <t>27.8</t>
+  </si>
+  <si>
+    <t>30.16.182</t>
+  </si>
+  <si>
+    <t>ESTILETE, CORPO PLÁSTICO, LÂMINA METAL LARGA (18MM), COM TRAVA DE SEGURANÇA, CORES VARIADAS.</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>30.16.2050</t>
+  </si>
+  <si>
+    <t>PINCEL MARCADOR PERMANENTE CD, MATERIAL PLÁSTICO, TIPO PONTA POLIÉSTER, COR TINTA VERMELHA, CARACTERÍSTICAS ADICIONAIS PONTA 2MM</t>
+  </si>
+  <si>
+    <t>1.25</t>
   </si>
   <si>
     <t>CADMAT</t>
@@ -1418,8 +1472,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00;(#,##0.00)"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -1491,7 +1546,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1520,7 +1575,7 @@
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="2" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="4" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
@@ -1529,12 +1584,13 @@
     <xf borderId="2" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -5997,6 +6053,191 @@
         <v>458</v>
       </c>
     </row>
+    <row r="174">
+      <c r="A174" s="2">
+        <v>45147.39012604167</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="F174" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H174" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I174" s="4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2">
+        <v>45147.39063577546</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="F175" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H175" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I175" s="4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2">
+        <v>45147.39105445602</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="F176" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H176" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I176" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2">
+        <v>45147.39149945602</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="F177" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H177" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I177" s="3">
+        <v>65.0</v>
+      </c>
+      <c r="N177" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2">
+        <v>45147.3919717824</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="F178" s="3">
+        <v>86.0</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H178" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I178" s="4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2">
+        <v>45147.39258770834</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="F179" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H179" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I179" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2">
+        <v>45147.39300671296</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="F180" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H180" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I180" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -6017,9 +6258,9 @@
   <cols>
     <col customWidth="1" min="1" max="4" width="18.88"/>
     <col customWidth="1" min="5" max="5" width="78.5"/>
-    <col customWidth="1" min="6" max="9" width="18.88"/>
-    <col customWidth="1" hidden="1" min="10" max="16" width="18.88"/>
-    <col customWidth="1" min="17" max="26" width="18.88"/>
+    <col customWidth="1" min="6" max="18" width="18.88"/>
+    <col customWidth="1" min="19" max="19" width="14.5"/>
+    <col customWidth="1" min="20" max="26" width="18.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -6069,16 +6310,16 @@
         <v>14</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>459</v>
+        <v>477</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>460</v>
+        <v>478</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>461</v>
+        <v>479</v>
       </c>
       <c r="T1" s="8" t="s">
-        <v>462</v>
+        <v>480</v>
       </c>
       <c r="U1" s="9" t="s">
         <v>7</v>
@@ -6087,16 +6328,16 @@
         <v>5</v>
       </c>
       <c r="W1" s="8" t="s">
-        <v>463</v>
+        <v>481</v>
       </c>
       <c r="X1" s="10" t="s">
-        <v>464</v>
+        <v>482</v>
       </c>
       <c r="Y1" s="11" t="s">
-        <v>465</v>
+        <v>483</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>464</v>
+        <v>482</v>
       </c>
     </row>
     <row r="2">
@@ -6118,11 +6359,15 @@
       <c r="G2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="13">
+      <c r="I2" s="13">
+        <v>0.43</v>
+      </c>
+      <c r="T2" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X2" s="15">
+        <f t="shared" ref="X2:X180" si="1">(F2*I2)</f>
+        <v>24.51</v>
       </c>
     </row>
     <row r="3">
@@ -6144,11 +6389,15 @@
       <c r="G3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T3" s="13">
+      <c r="I3" s="13">
+        <v>0.35</v>
+      </c>
+      <c r="T3" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X3" s="15">
+        <f t="shared" si="1"/>
+        <v>18.9</v>
       </c>
     </row>
     <row r="4">
@@ -6170,11 +6419,15 @@
       <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" s="13">
+      <c r="I4" s="13">
+        <v>1.09</v>
+      </c>
+      <c r="T4" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X4" s="15">
+        <f t="shared" si="1"/>
+        <v>33.79</v>
       </c>
     </row>
     <row r="5">
@@ -6196,11 +6449,15 @@
       <c r="G5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T5" s="13">
+      <c r="I5" s="13">
+        <v>1.21</v>
+      </c>
+      <c r="T5" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X5" s="15">
+        <f t="shared" si="1"/>
+        <v>79.86</v>
       </c>
     </row>
     <row r="6">
@@ -6222,11 +6479,15 @@
       <c r="G6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="T6" s="13">
+      <c r="I6" s="13">
+        <v>1.51</v>
+      </c>
+      <c r="T6" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X6" s="15">
+        <f t="shared" si="1"/>
+        <v>161.57</v>
       </c>
     </row>
     <row r="7">
@@ -6248,11 +6509,15 @@
       <c r="G7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="T7" s="13">
+      <c r="I7" s="13">
+        <v>0.18</v>
+      </c>
+      <c r="T7" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X7" s="15">
+        <f t="shared" si="1"/>
+        <v>69.48</v>
       </c>
     </row>
     <row r="8">
@@ -6274,11 +6539,15 @@
       <c r="G8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T8" s="13">
+      <c r="I8" s="13">
+        <v>0.39</v>
+      </c>
+      <c r="T8" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X8" s="15">
+        <f t="shared" si="1"/>
+        <v>117.39</v>
       </c>
     </row>
     <row r="9">
@@ -6300,11 +6569,15 @@
       <c r="G9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="T9" s="13">
+      <c r="I9" s="13">
+        <v>0.28</v>
+      </c>
+      <c r="T9" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X9" s="15">
+        <f t="shared" si="1"/>
+        <v>133.84</v>
       </c>
     </row>
     <row r="10">
@@ -6329,11 +6602,15 @@
       <c r="H10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T10" s="13">
+      <c r="I10" s="13">
+        <v>0.39</v>
+      </c>
+      <c r="T10" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X10" s="15">
+        <f t="shared" si="1"/>
+        <v>262.47</v>
       </c>
     </row>
     <row r="11">
@@ -6358,11 +6635,15 @@
       <c r="H11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="T11" s="13">
+      <c r="I11" s="13">
+        <v>0.42</v>
+      </c>
+      <c r="T11" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X11" s="15">
+        <f t="shared" si="1"/>
+        <v>109.2</v>
       </c>
     </row>
     <row r="12">
@@ -6387,11 +6668,15 @@
       <c r="H12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="T12" s="13">
+      <c r="I12" s="13">
+        <v>0.77</v>
+      </c>
+      <c r="T12" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X12" s="15">
+        <f t="shared" si="1"/>
+        <v>14.63</v>
       </c>
     </row>
     <row r="13">
@@ -6416,11 +6701,15 @@
       <c r="H13" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="T13" s="13">
+      <c r="I13" s="13">
+        <v>1.84</v>
+      </c>
+      <c r="T13" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X13" s="15">
+        <f t="shared" si="1"/>
+        <v>12.88</v>
       </c>
     </row>
     <row r="14">
@@ -6445,11 +6734,15 @@
       <c r="H14" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="T14" s="13">
+      <c r="I14" s="13">
+        <v>1.58</v>
+      </c>
+      <c r="T14" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X14" s="15">
+        <f t="shared" si="1"/>
+        <v>7.9</v>
       </c>
     </row>
     <row r="15">
@@ -6474,11 +6767,15 @@
       <c r="H15" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="T15" s="13">
+      <c r="I15" s="13">
+        <v>0.51</v>
+      </c>
+      <c r="T15" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X15" s="15">
+        <f t="shared" si="1"/>
+        <v>22.95</v>
       </c>
     </row>
     <row r="16">
@@ -6503,11 +6800,15 @@
       <c r="H16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="T16" s="13">
+      <c r="I16" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="T16" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X16" s="15">
+        <f t="shared" si="1"/>
+        <v>22.75</v>
       </c>
     </row>
     <row r="17">
@@ -6532,11 +6833,15 @@
       <c r="H17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="T17" s="13">
+      <c r="I17" s="13">
+        <v>3.1</v>
+      </c>
+      <c r="T17" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X17" s="15">
+        <f t="shared" si="1"/>
+        <v>24.8</v>
       </c>
     </row>
     <row r="18">
@@ -6561,11 +6866,15 @@
       <c r="H18" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I18" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="T18" s="13">
+      <c r="I18" s="13">
+        <v>3.12</v>
+      </c>
+      <c r="T18" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X18" s="15">
+        <f t="shared" si="1"/>
+        <v>62.4</v>
       </c>
     </row>
     <row r="19">
@@ -6590,11 +6899,15 @@
       <c r="H19" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="T19" s="13">
+      <c r="I19" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="T19" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X19" s="15">
+        <f t="shared" si="1"/>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
@@ -6616,14 +6929,18 @@
       <c r="G20" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I20" s="3" t="s">
-        <v>75</v>
+      <c r="I20" s="13">
+        <v>0.64</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T20" s="13">
+      <c r="T20" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X20" s="15">
+        <f t="shared" si="1"/>
+        <v>46.72</v>
       </c>
     </row>
     <row r="21">
@@ -6645,14 +6962,18 @@
       <c r="G21" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I21" s="3" t="s">
-        <v>79</v>
+      <c r="I21" s="13">
+        <v>2.39</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T21" s="13">
+      <c r="T21" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X21" s="15">
+        <f t="shared" si="1"/>
+        <v>4.78</v>
       </c>
     </row>
     <row r="22">
@@ -6674,11 +6995,15 @@
       <c r="G22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="T22" s="13">
+      <c r="I22" s="13">
+        <v>3.13</v>
+      </c>
+      <c r="T22" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X22" s="15">
+        <f t="shared" si="1"/>
+        <v>413.16</v>
       </c>
     </row>
     <row r="23">
@@ -6700,11 +7025,15 @@
       <c r="G23" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I23" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="T23" s="13">
+      <c r="I23" s="13">
+        <v>4.31</v>
+      </c>
+      <c r="T23" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X23" s="15">
+        <f t="shared" si="1"/>
+        <v>241.36</v>
       </c>
     </row>
     <row r="24">
@@ -6729,11 +7058,15 @@
       <c r="G24" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="T24" s="13">
+      <c r="I24" s="13">
+        <v>4.31</v>
+      </c>
+      <c r="T24" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X24" s="15">
+        <f t="shared" si="1"/>
+        <v>241.36</v>
       </c>
     </row>
     <row r="25">
@@ -6755,11 +7088,15 @@
       <c r="G25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="T25" s="13">
+      <c r="I25" s="13">
+        <v>15.89</v>
+      </c>
+      <c r="T25" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X25" s="15">
+        <f t="shared" si="1"/>
+        <v>95.34</v>
       </c>
     </row>
     <row r="26">
@@ -6784,11 +7121,15 @@
       <c r="G26" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="T26" s="13">
+      <c r="I26" s="13">
+        <v>15.89</v>
+      </c>
+      <c r="T26" s="14">
         <v>1.15610116E8</v>
+      </c>
+      <c r="X26" s="15">
+        <f t="shared" si="1"/>
+        <v>127.12</v>
       </c>
     </row>
     <row r="27">
@@ -6810,11 +7151,15 @@
       <c r="G27" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="T27" s="13">
+      <c r="I27" s="13">
+        <v>13.5</v>
+      </c>
+      <c r="T27" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X27" s="15">
+        <f t="shared" si="1"/>
+        <v>2659.5</v>
       </c>
     </row>
     <row r="28">
@@ -6836,11 +7181,15 @@
       <c r="G28" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I28" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="T28" s="13">
+      <c r="I28" s="13">
+        <v>12.02</v>
+      </c>
+      <c r="T28" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X28" s="15">
+        <f t="shared" si="1"/>
+        <v>757.26</v>
       </c>
     </row>
     <row r="29">
@@ -6862,11 +7211,15 @@
       <c r="G29" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="T29" s="13">
+      <c r="I29" s="13">
+        <v>7.17</v>
+      </c>
+      <c r="T29" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X29" s="15">
+        <f t="shared" si="1"/>
+        <v>222.27</v>
       </c>
     </row>
     <row r="30">
@@ -6888,11 +7241,15 @@
       <c r="G30" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I30" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="T30" s="13">
+      <c r="I30" s="13">
+        <v>150.3</v>
+      </c>
+      <c r="T30" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X30" s="15">
+        <f t="shared" si="1"/>
+        <v>10220.4</v>
       </c>
     </row>
     <row r="31">
@@ -6914,11 +7271,15 @@
       <c r="G31" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I31" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="T31" s="13">
+      <c r="I31" s="13">
+        <v>14.7</v>
+      </c>
+      <c r="T31" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X31" s="15">
+        <f t="shared" si="1"/>
+        <v>117.6</v>
       </c>
     </row>
     <row r="32">
@@ -6940,11 +7301,15 @@
       <c r="G32" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="T32" s="13">
+      <c r="I32" s="13">
+        <v>4.59</v>
+      </c>
+      <c r="T32" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X32" s="15">
+        <f t="shared" si="1"/>
+        <v>18.36</v>
       </c>
     </row>
     <row r="33">
@@ -6966,11 +7331,15 @@
       <c r="G33" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I33" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="T33" s="13">
+      <c r="I33" s="13">
+        <v>9.99</v>
+      </c>
+      <c r="T33" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X33" s="15">
+        <f t="shared" si="1"/>
+        <v>49.95</v>
       </c>
     </row>
     <row r="34">
@@ -6992,11 +7361,15 @@
       <c r="G34" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="T34" s="13">
+      <c r="I34" s="13">
+        <v>201.74</v>
+      </c>
+      <c r="T34" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X34" s="15">
+        <f t="shared" si="1"/>
+        <v>403.48</v>
       </c>
     </row>
     <row r="35">
@@ -7018,11 +7391,15 @@
       <c r="G35" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="13">
         <v>127.0</v>
       </c>
-      <c r="T35" s="13">
+      <c r="T35" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X35" s="15">
+        <f t="shared" si="1"/>
+        <v>2032</v>
       </c>
     </row>
     <row r="36">
@@ -7044,11 +7421,15 @@
       <c r="G36" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I36" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="T36" s="13">
+      <c r="I36" s="13">
+        <v>14.5</v>
+      </c>
+      <c r="T36" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X36" s="15">
+        <f t="shared" si="1"/>
+        <v>826.5</v>
       </c>
     </row>
     <row r="37">
@@ -7070,11 +7451,15 @@
       <c r="G37" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="T37" s="13">
+      <c r="I37" s="13">
+        <v>0.12</v>
+      </c>
+      <c r="T37" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X37" s="15">
+        <f t="shared" si="1"/>
+        <v>72</v>
       </c>
     </row>
     <row r="38">
@@ -7096,11 +7481,15 @@
       <c r="G38" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="13">
         <v>26.0</v>
       </c>
-      <c r="T38" s="13">
+      <c r="T38" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X38" s="15">
+        <f t="shared" si="1"/>
+        <v>26</v>
       </c>
     </row>
     <row r="39">
@@ -7122,14 +7511,18 @@
       <c r="G39" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I39" s="3" t="s">
-        <v>125</v>
+      <c r="I39" s="13">
+        <v>1.26</v>
       </c>
       <c r="N39" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T39" s="13">
+      <c r="T39" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X39" s="15">
+        <f t="shared" si="1"/>
+        <v>35.28</v>
       </c>
     </row>
     <row r="40">
@@ -7151,11 +7544,15 @@
       <c r="G40" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I40" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="T40" s="13">
+      <c r="I40" s="13">
+        <v>1.3</v>
+      </c>
+      <c r="T40" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X40" s="15">
+        <f t="shared" si="1"/>
+        <v>23.4</v>
       </c>
     </row>
     <row r="41">
@@ -7177,11 +7574,15 @@
       <c r="G41" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I41" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="T41" s="13">
+      <c r="I41" s="13">
+        <v>59.2</v>
+      </c>
+      <c r="T41" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X41" s="15">
+        <f t="shared" si="1"/>
+        <v>2664</v>
       </c>
     </row>
     <row r="42">
@@ -7203,14 +7604,18 @@
       <c r="G42" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I42" s="4" t="s">
-        <v>134</v>
+      <c r="I42" s="13">
+        <v>2.4</v>
       </c>
       <c r="N42" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T42" s="13">
+      <c r="T42" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X42" s="15">
+        <f t="shared" si="1"/>
+        <v>110.4</v>
       </c>
     </row>
     <row r="43">
@@ -7232,11 +7637,15 @@
       <c r="G43" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="T43" s="13">
+      <c r="I43" s="13">
+        <v>1.69</v>
+      </c>
+      <c r="T43" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X43" s="15">
+        <f t="shared" si="1"/>
+        <v>42.25</v>
       </c>
     </row>
     <row r="44">
@@ -7258,11 +7667,15 @@
       <c r="G44" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I44" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="T44" s="13">
+      <c r="I44" s="13">
+        <v>1.67</v>
+      </c>
+      <c r="T44" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X44" s="15">
+        <f t="shared" si="1"/>
+        <v>33.4</v>
       </c>
     </row>
     <row r="45">
@@ -7284,11 +7697,15 @@
       <c r="G45" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I45" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="T45" s="13">
+      <c r="I45" s="13">
+        <v>3.55</v>
+      </c>
+      <c r="T45" s="14">
         <v>1.15610128E8</v>
+      </c>
+      <c r="X45" s="15">
+        <f t="shared" si="1"/>
+        <v>63.9</v>
       </c>
     </row>
     <row r="46">
@@ -7310,11 +7727,15 @@
       <c r="G46" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I46" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="T46" s="13">
+      <c r="I46" s="13">
+        <v>6.29</v>
+      </c>
+      <c r="T46" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X46" s="15">
+        <f t="shared" si="1"/>
+        <v>125.8</v>
       </c>
     </row>
     <row r="47">
@@ -7336,11 +7757,15 @@
       <c r="G47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I47" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="T47" s="13">
+      <c r="I47" s="13">
+        <v>5.44</v>
+      </c>
+      <c r="T47" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X47" s="15">
+        <f t="shared" si="1"/>
+        <v>76.16</v>
       </c>
     </row>
     <row r="48">
@@ -7362,11 +7787,15 @@
       <c r="G48" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="T48" s="13">
-        <v>1.15610124E8</v>
+      <c r="I48" s="13">
+        <v>15.74</v>
+      </c>
+      <c r="T48" s="14">
+        <v>1.15610122E8</v>
+      </c>
+      <c r="X48" s="15">
+        <f t="shared" si="1"/>
+        <v>110.18</v>
       </c>
     </row>
     <row r="49">
@@ -7388,14 +7817,18 @@
       <c r="G49" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I49" s="3" t="s">
-        <v>155</v>
+      <c r="I49" s="13">
+        <v>7.48</v>
       </c>
       <c r="N49" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T49" s="13">
+      <c r="T49" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X49" s="15">
+        <f t="shared" si="1"/>
+        <v>792.88</v>
       </c>
     </row>
     <row r="50">
@@ -7417,14 +7850,18 @@
       <c r="G50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I50" s="3" t="s">
-        <v>158</v>
+      <c r="I50" s="13">
+        <v>11.87</v>
       </c>
       <c r="N50" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T50" s="13">
+      <c r="T50" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X50" s="15">
+        <f t="shared" si="1"/>
+        <v>273.01</v>
       </c>
     </row>
     <row r="51">
@@ -7446,11 +7883,15 @@
       <c r="G51" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="13">
         <v>15.0</v>
       </c>
-      <c r="T51" s="13">
+      <c r="T51" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X51" s="15">
+        <f t="shared" si="1"/>
+        <v>750</v>
       </c>
     </row>
     <row r="52">
@@ -7472,11 +7913,15 @@
       <c r="G52" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52" s="13">
         <v>6.0</v>
       </c>
-      <c r="T52" s="13">
+      <c r="T52" s="14">
         <v>1.15610126E8</v>
+      </c>
+      <c r="X52" s="15">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
     </row>
     <row r="53">
@@ -7498,11 +7943,15 @@
       <c r="G53" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I53" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="T53" s="13">
+      <c r="I53" s="13">
+        <v>4.8</v>
+      </c>
+      <c r="T53" s="14">
         <v>1.15610126E8</v>
+      </c>
+      <c r="X53" s="15">
+        <f t="shared" si="1"/>
+        <v>91.2</v>
       </c>
     </row>
     <row r="54">
@@ -7524,11 +7973,15 @@
       <c r="G54" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I54" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="T54" s="13">
+      <c r="I54" s="13">
+        <v>8.5</v>
+      </c>
+      <c r="T54" s="14">
         <v>1.15610128E8</v>
+      </c>
+      <c r="X54" s="15">
+        <f t="shared" si="1"/>
+        <v>127.5</v>
       </c>
     </row>
     <row r="55">
@@ -7550,11 +8003,15 @@
       <c r="G55" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I55" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="T55" s="13">
+      <c r="I55" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="T55" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X55" s="15">
+        <f t="shared" si="1"/>
+        <v>30</v>
       </c>
     </row>
     <row r="56">
@@ -7576,11 +8033,15 @@
       <c r="G56" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I56" s="13">
         <v>60.0</v>
       </c>
-      <c r="T56" s="13">
+      <c r="T56" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X56" s="15">
+        <f t="shared" si="1"/>
+        <v>180</v>
       </c>
     </row>
     <row r="57">
@@ -7602,11 +8063,15 @@
       <c r="G57" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I57" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="T57" s="13">
+      <c r="I57" s="13">
+        <v>1.85</v>
+      </c>
+      <c r="T57" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X57" s="15">
+        <f t="shared" si="1"/>
+        <v>606.8</v>
       </c>
     </row>
     <row r="58">
@@ -7628,11 +8093,15 @@
       <c r="G58" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I58" s="3">
+      <c r="I58" s="13">
         <v>52.0</v>
       </c>
-      <c r="T58" s="13">
+      <c r="T58" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X58" s="15">
+        <f t="shared" si="1"/>
+        <v>468</v>
       </c>
     </row>
     <row r="59">
@@ -7654,11 +8123,15 @@
       <c r="G59" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I59" s="3">
+      <c r="I59" s="13">
         <v>32.0</v>
       </c>
-      <c r="T59" s="13">
+      <c r="T59" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X59" s="15">
+        <f t="shared" si="1"/>
+        <v>256</v>
       </c>
     </row>
     <row r="60">
@@ -7680,11 +8153,15 @@
       <c r="G60" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I60" s="3">
+      <c r="I60" s="13">
         <v>54.0</v>
       </c>
-      <c r="T60" s="13">
+      <c r="T60" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X60" s="15">
+        <f t="shared" si="1"/>
+        <v>108</v>
       </c>
     </row>
     <row r="61">
@@ -7706,11 +8183,15 @@
       <c r="G61" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I61" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="T61" s="13">
+      <c r="I61" s="13">
+        <v>14.85</v>
+      </c>
+      <c r="T61" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X61" s="15">
+        <f t="shared" si="1"/>
+        <v>44.55</v>
       </c>
     </row>
     <row r="62">
@@ -7732,11 +8213,15 @@
       <c r="G62" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I62" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="T62" s="13">
+      <c r="I62" s="13">
+        <v>7.92</v>
+      </c>
+      <c r="T62" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X62" s="15">
+        <f t="shared" si="1"/>
+        <v>39.6</v>
       </c>
     </row>
     <row r="63">
@@ -7758,11 +8243,15 @@
       <c r="G63" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I63" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="T63" s="13">
+      <c r="I63" s="13">
+        <v>3.53</v>
+      </c>
+      <c r="T63" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X63" s="15">
+        <f t="shared" si="1"/>
+        <v>7.06</v>
       </c>
     </row>
     <row r="64">
@@ -7784,11 +8273,15 @@
       <c r="G64" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I64" s="3">
+      <c r="I64" s="13">
         <v>54.0</v>
       </c>
-      <c r="T64" s="13">
+      <c r="T64" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X64" s="15">
+        <f t="shared" si="1"/>
+        <v>918</v>
       </c>
     </row>
     <row r="65">
@@ -7810,11 +8303,15 @@
       <c r="G65" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I65" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="T65" s="13">
+      <c r="I65" s="13">
+        <v>51.48</v>
+      </c>
+      <c r="T65" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X65" s="15">
+        <f t="shared" si="1"/>
+        <v>514.8</v>
       </c>
     </row>
     <row r="66">
@@ -7836,11 +8333,15 @@
       <c r="G66" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I66" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="T66" s="13">
+      <c r="I66" s="13">
+        <v>99.86</v>
+      </c>
+      <c r="T66" s="14">
         <v>1.15610129E8</v>
+      </c>
+      <c r="X66" s="15">
+        <f t="shared" si="1"/>
+        <v>798.88</v>
       </c>
     </row>
     <row r="67">
@@ -7862,11 +8363,15 @@
       <c r="G67" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I67" s="3">
+      <c r="I67" s="13">
         <v>7.0</v>
       </c>
-      <c r="T67" s="13">
+      <c r="T67" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X67" s="15">
+        <f t="shared" si="1"/>
+        <v>21</v>
       </c>
     </row>
     <row r="68">
@@ -7888,11 +8393,15 @@
       <c r="G68" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I68" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="T68" s="13">
+      <c r="I68" s="13">
+        <v>0.32</v>
+      </c>
+      <c r="T68" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X68" s="15">
+        <f t="shared" si="1"/>
+        <v>22.4</v>
       </c>
     </row>
     <row r="69">
@@ -7914,11 +8423,15 @@
       <c r="G69" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I69" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="T69" s="13">
+      <c r="I69" s="13">
+        <v>12.66</v>
+      </c>
+      <c r="T69" s="14">
         <v>1.15610128E8</v>
+      </c>
+      <c r="X69" s="15">
+        <f t="shared" si="1"/>
+        <v>151.92</v>
       </c>
     </row>
     <row r="70">
@@ -7940,11 +8453,15 @@
       <c r="G70" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I70" s="3">
+      <c r="I70" s="13">
         <v>44.0</v>
       </c>
-      <c r="T70" s="13">
+      <c r="T70" s="14">
         <v>1.15610124E8</v>
+      </c>
+      <c r="X70" s="15">
+        <f t="shared" si="1"/>
+        <v>176</v>
       </c>
     </row>
     <row r="71">
@@ -7966,11 +8483,15 @@
       <c r="G71" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I71" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="T71" s="13">
+      <c r="I71" s="13">
+        <v>8.35</v>
+      </c>
+      <c r="T71" s="14">
         <v>1.15610126E8</v>
+      </c>
+      <c r="X71" s="15">
+        <f t="shared" si="1"/>
+        <v>83.5</v>
       </c>
     </row>
     <row r="72">
@@ -7992,11 +8513,15 @@
       <c r="G72" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I72" s="3">
+      <c r="I72" s="13">
         <v>1778.0</v>
       </c>
-      <c r="T72" s="13">
+      <c r="T72" s="14">
         <v>1.15610122E8</v>
+      </c>
+      <c r="X72" s="15">
+        <f t="shared" si="1"/>
+        <v>1778</v>
       </c>
     </row>
     <row r="73">
@@ -8018,10 +8543,16 @@
       <c r="G73" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I73" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="T73" s="14"/>
+      <c r="I73" s="13">
+        <v>17.9</v>
+      </c>
+      <c r="T73" s="14">
+        <v>1.15610114E8</v>
+      </c>
+      <c r="X73" s="15">
+        <f t="shared" si="1"/>
+        <v>1790</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="2">
@@ -8042,10 +8573,16 @@
       <c r="G74" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I74" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="T74" s="14"/>
+      <c r="I74" s="13">
+        <v>12.41</v>
+      </c>
+      <c r="T74" s="14">
+        <v>1.15610114E8</v>
+      </c>
+      <c r="X74" s="15">
+        <f t="shared" si="1"/>
+        <v>297.84</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="2">
@@ -8066,10 +8603,16 @@
       <c r="G75" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I75" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="T75" s="14"/>
+      <c r="I75" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="T75" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X75" s="15">
+        <f t="shared" si="1"/>
+        <v>1229.3</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="2">
@@ -8090,10 +8633,16 @@
       <c r="G76" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I76" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="T76" s="14"/>
+      <c r="I76" s="13">
+        <v>1.71</v>
+      </c>
+      <c r="T76" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X76" s="15">
+        <f t="shared" si="1"/>
+        <v>584.82</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="2">
@@ -8114,10 +8663,16 @@
       <c r="G77" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I77" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="T77" s="14"/>
+      <c r="I77" s="13">
+        <v>16.23</v>
+      </c>
+      <c r="T77" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X77" s="15">
+        <f t="shared" si="1"/>
+        <v>113.61</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="2">
@@ -8138,10 +8693,16 @@
       <c r="G78" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I78" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="T78" s="14"/>
+      <c r="I78" s="13">
+        <v>88.34</v>
+      </c>
+      <c r="T78" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X78" s="15">
+        <f t="shared" si="1"/>
+        <v>1060.08</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="2">
@@ -8165,10 +8726,16 @@
       <c r="G79" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I79" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="T79" s="14"/>
+      <c r="I79" s="13">
+        <v>16.23</v>
+      </c>
+      <c r="T79" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X79" s="15">
+        <f t="shared" si="1"/>
+        <v>113.61</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="2">
@@ -8192,10 +8759,16 @@
       <c r="G80" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I80" s="3">
+      <c r="I80" s="13">
         <v>52.0</v>
       </c>
-      <c r="T80" s="14"/>
+      <c r="T80" s="14">
+        <v>1.15610122E8</v>
+      </c>
+      <c r="X80" s="15">
+        <f t="shared" si="1"/>
+        <v>468</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="2">
@@ -8216,10 +8789,16 @@
       <c r="G81" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I81" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="T81" s="14"/>
+      <c r="I81" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="T81" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X81" s="15">
+        <f t="shared" si="1"/>
+        <v>10.35</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="2">
@@ -8240,10 +8819,16 @@
       <c r="G82" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I82" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="T82" s="14"/>
+      <c r="I82" s="13">
+        <v>0.68</v>
+      </c>
+      <c r="T82" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X82" s="15">
+        <f t="shared" si="1"/>
+        <v>25.84</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="2">
@@ -8264,10 +8849,16 @@
       <c r="G83" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I83" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T83" s="14"/>
+      <c r="I83" s="13">
+        <v>0.35</v>
+      </c>
+      <c r="T83" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X83" s="15">
+        <f t="shared" si="1"/>
+        <v>50.75</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="2">
@@ -8288,10 +8879,16 @@
       <c r="G84" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I84" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T84" s="14"/>
+      <c r="I84" s="13">
+        <v>0.35</v>
+      </c>
+      <c r="T84" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X84" s="15">
+        <f t="shared" si="1"/>
+        <v>104.65</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="2">
@@ -8312,10 +8909,16 @@
       <c r="G85" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I85" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="T85" s="14"/>
+      <c r="I85" s="13">
+        <v>1.31</v>
+      </c>
+      <c r="T85" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X85" s="15">
+        <f t="shared" si="1"/>
+        <v>35.37</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="2">
@@ -8336,10 +8939,16 @@
       <c r="G86" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I86" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="T86" s="14"/>
+      <c r="I86" s="13">
+        <v>2.5</v>
+      </c>
+      <c r="T86" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X86" s="15">
+        <f t="shared" si="1"/>
+        <v>37.5</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="2">
@@ -8360,10 +8969,16 @@
       <c r="G87" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I87" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="T87" s="14"/>
+      <c r="I87" s="13">
+        <v>3.22</v>
+      </c>
+      <c r="T87" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X87" s="15">
+        <f t="shared" si="1"/>
+        <v>244.72</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="2">
@@ -8384,10 +8999,16 @@
       <c r="G88" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I88" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="T88" s="14"/>
+      <c r="I88" s="13">
+        <v>5.97</v>
+      </c>
+      <c r="T88" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X88" s="15">
+        <f t="shared" si="1"/>
+        <v>125.37</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="2">
@@ -8408,10 +9029,16 @@
       <c r="G89" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I89" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="T89" s="14"/>
+      <c r="I89" s="13">
+        <v>22.3</v>
+      </c>
+      <c r="T89" s="14">
+        <v>1.15610128E8</v>
+      </c>
+      <c r="X89" s="15">
+        <f t="shared" si="1"/>
+        <v>200.7</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="2">
@@ -8432,10 +9059,16 @@
       <c r="G90" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I90" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="T90" s="14"/>
+      <c r="I90" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="T90" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X90" s="15">
+        <f t="shared" si="1"/>
+        <v>7.8</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="2">
@@ -8456,10 +9089,16 @@
       <c r="G91" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I91" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="T91" s="14"/>
+      <c r="I91" s="13">
+        <v>0.66</v>
+      </c>
+      <c r="T91" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X91" s="15">
+        <f t="shared" si="1"/>
+        <v>13.2</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="2">
@@ -8480,10 +9119,16 @@
       <c r="G92" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I92" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="T92" s="14"/>
+      <c r="I92" s="13">
+        <v>0.85</v>
+      </c>
+      <c r="T92" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X92" s="15">
+        <f t="shared" si="1"/>
+        <v>5.95</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="2">
@@ -8504,10 +9149,16 @@
       <c r="G93" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I93" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="T93" s="14"/>
+      <c r="I93" s="13">
+        <v>0.65</v>
+      </c>
+      <c r="T93" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X93" s="15">
+        <f t="shared" si="1"/>
+        <v>14.95</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="2">
@@ -8528,10 +9179,16 @@
       <c r="G94" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I94" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="T94" s="14"/>
+      <c r="I94" s="13">
+        <v>0.45</v>
+      </c>
+      <c r="T94" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X94" s="15">
+        <f t="shared" si="1"/>
+        <v>4.05</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="2">
@@ -8552,10 +9209,16 @@
       <c r="G95" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I95" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="T95" s="14"/>
+      <c r="I95" s="13">
+        <v>7.99</v>
+      </c>
+      <c r="T95" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X95" s="15">
+        <f t="shared" si="1"/>
+        <v>23.97</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="2">
@@ -8576,10 +9239,16 @@
       <c r="G96" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I96" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="T96" s="14"/>
+      <c r="I96" s="13">
+        <v>5.09</v>
+      </c>
+      <c r="T96" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X96" s="15">
+        <f t="shared" si="1"/>
+        <v>20.36</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="2">
@@ -8600,10 +9269,16 @@
       <c r="G97" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I97" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="T97" s="14"/>
+      <c r="I97" s="13">
+        <v>7.7</v>
+      </c>
+      <c r="T97" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X97" s="15">
+        <f t="shared" si="1"/>
+        <v>69.3</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="2">
@@ -8627,10 +9302,16 @@
       <c r="G98" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I98" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="T98" s="14"/>
+      <c r="I98" s="13">
+        <v>7.99</v>
+      </c>
+      <c r="T98" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X98" s="15">
+        <f t="shared" si="1"/>
+        <v>23.97</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="2">
@@ -8651,10 +9332,16 @@
       <c r="G99" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I99" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="T99" s="14"/>
+      <c r="I99" s="13">
+        <v>4.38</v>
+      </c>
+      <c r="T99" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X99" s="15">
+        <f t="shared" si="1"/>
+        <v>205.86</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="2">
@@ -8675,10 +9362,16 @@
       <c r="G100" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I100" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="T100" s="14"/>
+      <c r="I100" s="13">
+        <v>1.94</v>
+      </c>
+      <c r="T100" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X100" s="15">
+        <f t="shared" si="1"/>
+        <v>44.62</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="2">
@@ -8699,10 +9392,16 @@
       <c r="G101" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I101" s="3">
+      <c r="I101" s="13">
         <v>15.0</v>
       </c>
-      <c r="T101" s="14"/>
+      <c r="T101" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X101" s="15">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="2">
@@ -8723,10 +9422,16 @@
       <c r="G102" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I102" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="T102" s="14"/>
+      <c r="I102" s="13">
+        <v>5.6</v>
+      </c>
+      <c r="T102" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X102" s="15">
+        <f t="shared" si="1"/>
+        <v>44.8</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="2">
@@ -8747,10 +9452,16 @@
       <c r="G103" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I103" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="T103" s="14"/>
+      <c r="I103" s="13">
+        <v>15.89</v>
+      </c>
+      <c r="T103" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X103" s="15">
+        <f t="shared" si="1"/>
+        <v>15.89</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="2">
@@ -8771,10 +9482,16 @@
       <c r="G104" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I104" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="T104" s="14"/>
+      <c r="I104" s="13">
+        <v>7.2</v>
+      </c>
+      <c r="T104" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X104" s="15">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="2">
@@ -8795,13 +9512,19 @@
       <c r="G105" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I105" s="3" t="s">
-        <v>298</v>
+      <c r="I105" s="13">
+        <v>3.65</v>
       </c>
       <c r="L105" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T105" s="14"/>
+      <c r="T105" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X105" s="15">
+        <f t="shared" si="1"/>
+        <v>3.65</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="2">
@@ -8822,10 +9545,16 @@
       <c r="G106" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I106" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="T106" s="14"/>
+      <c r="I106" s="13">
+        <v>4.23</v>
+      </c>
+      <c r="T106" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X106" s="15">
+        <f t="shared" si="1"/>
+        <v>50.76</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="2">
@@ -8846,10 +9575,16 @@
       <c r="G107" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I107" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="T107" s="14"/>
+      <c r="I107" s="13">
+        <v>17.01</v>
+      </c>
+      <c r="T107" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X107" s="15">
+        <f t="shared" si="1"/>
+        <v>136.08</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="2">
@@ -8870,10 +9605,16 @@
       <c r="G108" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I108" s="3">
+      <c r="I108" s="13">
         <v>15.0</v>
       </c>
-      <c r="T108" s="14"/>
+      <c r="T108" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X108" s="15">
+        <f t="shared" si="1"/>
+        <v>135</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="2">
@@ -8894,10 +9635,16 @@
       <c r="G109" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I109" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="T109" s="14"/>
+      <c r="I109" s="13">
+        <v>0.07</v>
+      </c>
+      <c r="T109" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X109" s="15">
+        <f t="shared" si="1"/>
+        <v>16.1</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="2">
@@ -8918,10 +9665,16 @@
       <c r="G110" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I110" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="T110" s="14"/>
+      <c r="I110" s="13">
+        <v>0.08</v>
+      </c>
+      <c r="T110" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X110" s="15">
+        <f t="shared" si="1"/>
+        <v>84.08</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="2">
@@ -8945,10 +9698,16 @@
       <c r="G111" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I111" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="T111" s="14"/>
+      <c r="I111" s="13">
+        <v>0.68</v>
+      </c>
+      <c r="T111" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X111" s="15">
+        <f t="shared" si="1"/>
+        <v>27.88</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="2">
@@ -8969,10 +9728,16 @@
       <c r="G112" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I112" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="T112" s="14"/>
+      <c r="I112" s="13">
+        <v>13.58</v>
+      </c>
+      <c r="T112" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X112" s="15">
+        <f t="shared" si="1"/>
+        <v>81.48</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="2">
@@ -8993,10 +9758,16 @@
       <c r="G113" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I113" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="T113" s="14"/>
+      <c r="I113" s="13">
+        <v>1.42</v>
+      </c>
+      <c r="T113" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X113" s="15">
+        <f t="shared" si="1"/>
+        <v>710</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="2">
@@ -9017,10 +9788,16 @@
       <c r="G114" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I114" s="4" t="s">
-        <v>321</v>
-      </c>
-      <c r="T114" s="14"/>
+      <c r="I114" s="13">
+        <v>2.06</v>
+      </c>
+      <c r="T114" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X114" s="15">
+        <f t="shared" si="1"/>
+        <v>24.72</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="2">
@@ -9041,10 +9818,16 @@
       <c r="G115" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I115" s="3">
+      <c r="I115" s="13">
         <v>4.0</v>
       </c>
-      <c r="T115" s="14"/>
+      <c r="T115" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X115" s="15">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="2">
@@ -9065,10 +9848,16 @@
       <c r="G116" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I116" s="3" t="s">
-        <v>326</v>
-      </c>
-      <c r="T116" s="14"/>
+      <c r="I116" s="13">
+        <v>3.54</v>
+      </c>
+      <c r="T116" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X116" s="15">
+        <f t="shared" si="1"/>
+        <v>10.62</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="2">
@@ -9089,10 +9878,16 @@
       <c r="G117" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I117" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="T117" s="14"/>
+      <c r="I117" s="13">
+        <v>2.3</v>
+      </c>
+      <c r="T117" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X117" s="15">
+        <f t="shared" si="1"/>
+        <v>140.3</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="2">
@@ -9113,10 +9908,16 @@
       <c r="G118" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I118" s="3" t="s">
-        <v>332</v>
-      </c>
-      <c r="T118" s="14"/>
+      <c r="I118" s="13">
+        <v>23.16</v>
+      </c>
+      <c r="T118" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X118" s="15">
+        <f t="shared" si="1"/>
+        <v>138.96</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="2">
@@ -9137,10 +9938,16 @@
       <c r="G119" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I119" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="T119" s="14"/>
+      <c r="I119" s="13">
+        <v>81.39</v>
+      </c>
+      <c r="T119" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X119" s="15">
+        <f t="shared" si="1"/>
+        <v>895.29</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="2">
@@ -9164,10 +9971,16 @@
       <c r="G120" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I120" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="T120" s="14"/>
+      <c r="I120" s="13">
+        <v>0.95</v>
+      </c>
+      <c r="T120" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X120" s="15">
+        <f t="shared" si="1"/>
+        <v>1088.7</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="2">
@@ -9188,10 +10001,16 @@
       <c r="G121" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I121" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="T121" s="14"/>
+      <c r="I121" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="T121" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X121" s="15">
+        <f t="shared" si="1"/>
+        <v>1.8</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="2">
@@ -9212,10 +10031,16 @@
       <c r="G122" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I122" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="T122" s="14"/>
+      <c r="I122" s="13">
+        <v>1.08</v>
+      </c>
+      <c r="T122" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X122" s="15">
+        <f t="shared" si="1"/>
+        <v>33.48</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="2">
@@ -9236,10 +10061,16 @@
       <c r="G123" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I123" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="T123" s="14"/>
+      <c r="I123" s="13">
+        <v>7.52</v>
+      </c>
+      <c r="T123" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X123" s="15">
+        <f t="shared" si="1"/>
+        <v>323.36</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="2">
@@ -9260,10 +10091,16 @@
       <c r="G124" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I124" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="T124" s="14"/>
+      <c r="I124" s="13">
+        <v>7.78</v>
+      </c>
+      <c r="T124" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X124" s="15">
+        <f t="shared" si="1"/>
+        <v>342.32</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="2">
@@ -9287,10 +10124,16 @@
       <c r="H125" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I125" s="4" t="s">
-        <v>341</v>
-      </c>
-      <c r="T125" s="14"/>
+      <c r="I125" s="13">
+        <v>1.08</v>
+      </c>
+      <c r="T125" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X125" s="15">
+        <f t="shared" si="1"/>
+        <v>28.08</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="2">
@@ -9317,10 +10160,16 @@
       <c r="H126" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I126" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="T126" s="14"/>
+      <c r="I126" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="T126" s="14">
+        <v>1.15610124E8</v>
+      </c>
+      <c r="X126" s="15">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="2">
@@ -9344,10 +10193,16 @@
       <c r="H127" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I127" s="3" t="s">
-        <v>352</v>
-      </c>
-      <c r="T127" s="14"/>
+      <c r="I127" s="13">
+        <v>17.95</v>
+      </c>
+      <c r="T127" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X127" s="15">
+        <f t="shared" si="1"/>
+        <v>107.7</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="2">
@@ -9371,10 +10226,16 @@
       <c r="H128" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I128" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="T128" s="14"/>
+      <c r="I128" s="13">
+        <v>11.11</v>
+      </c>
+      <c r="T128" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X128" s="15">
+        <f t="shared" si="1"/>
+        <v>55.55</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="2">
@@ -9398,10 +10259,16 @@
       <c r="H129" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I129" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="T129" s="14"/>
+      <c r="I129" s="13">
+        <v>16.33</v>
+      </c>
+      <c r="T129" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X129" s="15">
+        <f t="shared" si="1"/>
+        <v>2857.75</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="2">
@@ -9425,10 +10292,16 @@
       <c r="H130" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I130" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="T130" s="14"/>
+      <c r="I130" s="13">
+        <v>21.78</v>
+      </c>
+      <c r="T130" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X130" s="15">
+        <f t="shared" si="1"/>
+        <v>871.2</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="2">
@@ -9452,10 +10325,16 @@
       <c r="H131" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I131" s="3">
+      <c r="I131" s="13">
         <v>65.0</v>
       </c>
-      <c r="T131" s="14"/>
+      <c r="T131" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X131" s="15">
+        <f t="shared" si="1"/>
+        <v>455</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="2">
@@ -9479,10 +10358,16 @@
       <c r="H132" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I132" s="3">
+      <c r="I132" s="13">
         <v>65.0</v>
       </c>
-      <c r="T132" s="14"/>
+      <c r="T132" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X132" s="15">
+        <f t="shared" si="1"/>
+        <v>650</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="2">
@@ -9506,10 +10391,16 @@
       <c r="H133" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I133" s="3">
+      <c r="I133" s="13">
         <v>65.0</v>
       </c>
-      <c r="T133" s="14"/>
+      <c r="T133" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X133" s="15">
+        <f t="shared" si="1"/>
+        <v>715</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="2">
@@ -9533,10 +10424,16 @@
       <c r="H134" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I134" s="3">
+      <c r="I134" s="13">
         <v>65.0</v>
       </c>
-      <c r="T134" s="14"/>
+      <c r="T134" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X134" s="15">
+        <f t="shared" si="1"/>
+        <v>715</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="2">
@@ -9560,10 +10457,16 @@
       <c r="H135" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I135" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="T135" s="14"/>
+      <c r="I135" s="13">
+        <v>54.99</v>
+      </c>
+      <c r="T135" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X135" s="15">
+        <f t="shared" si="1"/>
+        <v>1099.8</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="2">
@@ -9587,10 +10490,16 @@
       <c r="H136" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I136" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="T136" s="14"/>
+      <c r="I136" s="13">
+        <v>8.7</v>
+      </c>
+      <c r="T136" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X136" s="15">
+        <f t="shared" si="1"/>
+        <v>174</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="2">
@@ -9614,10 +10523,16 @@
       <c r="H137" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I137" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="T137" s="14"/>
+      <c r="I137" s="13">
+        <v>67.5</v>
+      </c>
+      <c r="T137" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X137" s="15">
+        <f t="shared" si="1"/>
+        <v>405</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="2">
@@ -9644,10 +10559,16 @@
       <c r="H138" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I138" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="T138" s="14"/>
+      <c r="I138" s="13">
+        <v>67.5</v>
+      </c>
+      <c r="T138" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X138" s="15">
+        <f t="shared" si="1"/>
+        <v>337.5</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="2">
@@ -9671,10 +10592,16 @@
       <c r="H139" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I139" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="T139" s="14"/>
+      <c r="I139" s="13">
+        <v>8.75</v>
+      </c>
+      <c r="T139" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X139" s="15">
+        <f t="shared" si="1"/>
+        <v>26.25</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="2">
@@ -9698,10 +10625,16 @@
       <c r="H140" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I140" s="3">
+      <c r="I140" s="13">
         <v>8.0</v>
       </c>
-      <c r="T140" s="14"/>
+      <c r="T140" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X140" s="15">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="2">
@@ -9725,10 +10658,16 @@
       <c r="H141" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I141" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="T141" s="14"/>
+      <c r="I141" s="13">
+        <v>8.1</v>
+      </c>
+      <c r="T141" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X141" s="15">
+        <f t="shared" si="1"/>
+        <v>1215</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="2">
@@ -9752,10 +10691,16 @@
       <c r="H142" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I142" s="3">
+      <c r="I142" s="13">
         <v>40.0</v>
       </c>
-      <c r="T142" s="14"/>
+      <c r="T142" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X142" s="15">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="2">
@@ -9779,10 +10724,16 @@
       <c r="H143" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I143" s="3">
+      <c r="I143" s="13">
         <v>25.0</v>
       </c>
-      <c r="T143" s="14"/>
+      <c r="T143" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X143" s="15">
+        <f t="shared" si="1"/>
+        <v>1275</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="2">
@@ -9806,10 +10757,16 @@
       <c r="H144" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I144" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="T144" s="14"/>
+      <c r="I144" s="13">
+        <v>17.59</v>
+      </c>
+      <c r="T144" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X144" s="15">
+        <f t="shared" si="1"/>
+        <v>738.78</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="2">
@@ -9833,10 +10790,16 @@
       <c r="H145" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I145" s="4" t="s">
-        <v>397</v>
-      </c>
-      <c r="T145" s="14"/>
+      <c r="I145" s="13">
+        <v>29.3</v>
+      </c>
+      <c r="T145" s="14">
+        <v>1.15610126E8</v>
+      </c>
+      <c r="X145" s="15">
+        <f t="shared" si="1"/>
+        <v>117.2</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="2">
@@ -9860,10 +10823,16 @@
       <c r="H146" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I146" s="3">
+      <c r="I146" s="13">
         <v>37.0</v>
       </c>
-      <c r="T146" s="14"/>
+      <c r="T146" s="14">
+        <v>1.15610126E8</v>
+      </c>
+      <c r="X146" s="15">
+        <f t="shared" si="1"/>
+        <v>148</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="2">
@@ -9887,10 +10856,16 @@
       <c r="H147" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I147" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="T147" s="14"/>
+      <c r="I147" s="13">
+        <v>117.25</v>
+      </c>
+      <c r="T147" s="14">
+        <v>1.15610114E8</v>
+      </c>
+      <c r="X147" s="15">
+        <f t="shared" si="1"/>
+        <v>469</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="2">
@@ -9914,10 +10889,16 @@
       <c r="H148" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I148" s="3" t="s">
-        <v>405</v>
-      </c>
-      <c r="T148" s="14"/>
+      <c r="I148" s="13">
+        <v>15.36</v>
+      </c>
+      <c r="T148" s="14">
+        <v>1.15610114E8</v>
+      </c>
+      <c r="X148" s="15">
+        <f t="shared" si="1"/>
+        <v>61.44</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="2">
@@ -9941,10 +10922,16 @@
       <c r="H149" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I149" s="3">
+      <c r="I149" s="13">
         <v>170.0</v>
       </c>
-      <c r="T149" s="14"/>
+      <c r="T149" s="14">
+        <v>1.15610114E8</v>
+      </c>
+      <c r="X149" s="15">
+        <f t="shared" si="1"/>
+        <v>340</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="2">
@@ -9968,10 +10955,16 @@
       <c r="H150" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I150" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="T150" s="14"/>
+      <c r="I150" s="13">
+        <v>29.58</v>
+      </c>
+      <c r="T150" s="14">
+        <v>1.15610114E8</v>
+      </c>
+      <c r="X150" s="15">
+        <f t="shared" si="1"/>
+        <v>118.32</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="2">
@@ -9995,10 +10988,16 @@
       <c r="H151" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I151" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="T151" s="14"/>
+      <c r="I151" s="13">
+        <v>66.24</v>
+      </c>
+      <c r="T151" s="14">
+        <v>1.15610114E8</v>
+      </c>
+      <c r="X151" s="15">
+        <f t="shared" si="1"/>
+        <v>264.96</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="2">
@@ -10022,10 +11021,16 @@
       <c r="H152" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I152" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="T152" s="14"/>
+      <c r="I152" s="13">
+        <v>98.23</v>
+      </c>
+      <c r="T152" s="14">
+        <v>1.15610114E8</v>
+      </c>
+      <c r="X152" s="15">
+        <f t="shared" si="1"/>
+        <v>392.92</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="2">
@@ -10049,13 +11054,19 @@
       <c r="H153" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I153" s="3">
+      <c r="I153" s="13">
         <v>65.0</v>
       </c>
       <c r="N153" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="T153" s="14"/>
+      <c r="T153" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X153" s="15">
+        <f t="shared" si="1"/>
+        <v>975</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="2">
@@ -10079,10 +11090,16 @@
       <c r="H154" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I154" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="T154" s="14"/>
+      <c r="I154" s="13">
+        <v>323.22</v>
+      </c>
+      <c r="T154" s="14">
+        <v>1.15610126E8</v>
+      </c>
+      <c r="X154" s="15">
+        <f t="shared" si="1"/>
+        <v>3878.64</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="2">
@@ -10106,10 +11123,16 @@
       <c r="H155" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I155" s="3">
+      <c r="I155" s="13">
         <v>34.0</v>
       </c>
-      <c r="T155" s="14"/>
+      <c r="T155" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X155" s="15">
+        <f t="shared" si="1"/>
+        <v>136</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="2">
@@ -10133,10 +11156,16 @@
       <c r="H156" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I156" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="T156" s="14"/>
+      <c r="I156" s="13">
+        <v>28.06</v>
+      </c>
+      <c r="T156" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X156" s="15">
+        <f t="shared" si="1"/>
+        <v>84.18</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="2">
@@ -10160,10 +11189,16 @@
       <c r="H157" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I157" s="4" t="s">
-        <v>427</v>
-      </c>
-      <c r="T157" s="14"/>
+      <c r="I157" s="13">
+        <v>7.1</v>
+      </c>
+      <c r="T157" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X157" s="15">
+        <f t="shared" si="1"/>
+        <v>35.5</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="2">
@@ -10187,10 +11222,16 @@
       <c r="H158" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I158" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="T158" s="14"/>
+      <c r="I158" s="13">
+        <v>81.45</v>
+      </c>
+      <c r="T158" s="14">
+        <v>1.15610129E8</v>
+      </c>
+      <c r="X158" s="15">
+        <f t="shared" si="1"/>
+        <v>325.8</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="2">
@@ -10214,10 +11255,16 @@
       <c r="H159" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I159" s="3">
+      <c r="I159" s="13">
         <v>65.0</v>
       </c>
-      <c r="T159" s="14"/>
+      <c r="T159" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X159" s="15">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="2">
@@ -10241,10 +11288,16 @@
       <c r="H160" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I160" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="T160" s="14"/>
+      <c r="I160" s="13">
+        <v>1.8</v>
+      </c>
+      <c r="T160" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X160" s="15">
+        <f t="shared" si="1"/>
+        <v>19.8</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="2">
@@ -10268,10 +11321,16 @@
       <c r="H161" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I161" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="T161" s="14"/>
+      <c r="I161" s="13">
+        <v>54.99</v>
+      </c>
+      <c r="T161" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X161" s="15">
+        <f t="shared" si="1"/>
+        <v>1099.8</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="2">
@@ -10295,10 +11354,16 @@
       <c r="H162" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I162" s="3">
+      <c r="I162" s="13">
         <v>20.0</v>
       </c>
-      <c r="T162" s="14"/>
+      <c r="T162" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X162" s="15">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="2">
@@ -10322,10 +11387,16 @@
       <c r="H163" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I163" s="3">
+      <c r="I163" s="13">
         <v>60.0</v>
       </c>
-      <c r="T163" s="14"/>
+      <c r="T163" s="14">
+        <v>1.15610142E8</v>
+      </c>
+      <c r="X163" s="15">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="2">
@@ -10349,10 +11420,16 @@
       <c r="H164" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I164" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="T164" s="14"/>
+      <c r="I164" s="13">
+        <v>0.49</v>
+      </c>
+      <c r="T164" s="14">
+        <v>1.15610124E8</v>
+      </c>
+      <c r="X164" s="15">
+        <f t="shared" si="1"/>
+        <v>245</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="2">
@@ -10379,10 +11456,16 @@
       <c r="H165" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I165" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="T165" s="14"/>
+      <c r="I165" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="T165" s="14">
+        <v>1.15610124E8</v>
+      </c>
+      <c r="X165" s="15">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="2">
@@ -10406,10 +11489,16 @@
       <c r="H166" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I166" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="T166" s="14"/>
+      <c r="I166" s="13">
+        <v>0.19</v>
+      </c>
+      <c r="T166" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X166" s="15">
+        <f t="shared" si="1"/>
+        <v>164.35</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="2">
@@ -10433,10 +11522,16 @@
       <c r="H167" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I167" s="3" t="s">
-        <v>413</v>
-      </c>
-      <c r="T167" s="14"/>
+      <c r="I167" s="13">
+        <v>66.24</v>
+      </c>
+      <c r="T167" s="14">
+        <v>1.15610114E8</v>
+      </c>
+      <c r="X167" s="15">
+        <f t="shared" si="1"/>
+        <v>264.96</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="2">
@@ -10460,10 +11555,16 @@
       <c r="H168" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I168" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="T168" s="14"/>
+      <c r="I168" s="13">
+        <v>20.43</v>
+      </c>
+      <c r="T168" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X168" s="15">
+        <f t="shared" si="1"/>
+        <v>388.17</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="2">
@@ -10487,10 +11588,16 @@
       <c r="H169" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I169" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="T169" s="14"/>
+      <c r="I169" s="13">
+        <v>14.79</v>
+      </c>
+      <c r="T169" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X169" s="15">
+        <f t="shared" si="1"/>
+        <v>88.74</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="2">
@@ -10514,10 +11621,16 @@
       <c r="H170" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I170" s="4" t="s">
-        <v>449</v>
-      </c>
-      <c r="T170" s="14"/>
+      <c r="I170" s="13">
+        <v>3.6</v>
+      </c>
+      <c r="T170" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X170" s="15">
+        <f t="shared" si="1"/>
+        <v>32.4</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="2">
@@ -10541,10 +11654,16 @@
       <c r="H171" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I171" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="T171" s="14"/>
+      <c r="I171" s="13">
+        <v>1.62</v>
+      </c>
+      <c r="T171" s="14">
+        <v>1.15610123E8</v>
+      </c>
+      <c r="X171" s="15">
+        <f t="shared" si="1"/>
+        <v>69.66</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="2">
@@ -10568,10 +11687,16 @@
       <c r="H172" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I172" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="T172" s="14"/>
+      <c r="I172" s="13">
+        <v>28.55</v>
+      </c>
+      <c r="T172" s="14">
+        <v>1.15610122E8</v>
+      </c>
+      <c r="X172" s="15">
+        <f t="shared" si="1"/>
+        <v>485.35</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="2">
@@ -10595,13 +11720,253 @@
       <c r="H173" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I173" s="3" t="s">
-        <v>458</v>
-      </c>
-      <c r="T173" s="14"/>
+      <c r="I173" s="13">
+        <v>10.75</v>
+      </c>
+      <c r="T173" s="14">
+        <v>1.15610123E8</v>
+      </c>
+      <c r="X173" s="15">
+        <f t="shared" si="1"/>
+        <v>18758.75</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2">
+        <v>45147.39012604167</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="F174" s="3">
+        <v>12.0</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H174" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I174" s="13">
+        <v>2.09</v>
+      </c>
+      <c r="T174" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X174" s="15">
+        <f t="shared" si="1"/>
+        <v>25.08</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2">
+        <v>45147.39063577546</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="F175" s="3">
+        <v>5.0</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H175" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I175" s="13">
+        <v>9.8</v>
+      </c>
+      <c r="T175" s="14">
+        <v>1.15610144E8</v>
+      </c>
+      <c r="X175" s="15">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2">
+        <v>45147.39105445602</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="F176" s="3">
+        <v>4.0</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H176" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I176" s="13">
+        <v>21.89</v>
+      </c>
+      <c r="T176" s="14">
+        <v>1.15610144E8</v>
+      </c>
+      <c r="X176" s="15">
+        <f t="shared" si="1"/>
+        <v>87.56</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2">
+        <v>45147.39149945602</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="F177" s="3">
+        <v>15.0</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H177" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I177" s="13">
+        <v>65.0</v>
+      </c>
+      <c r="N177" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="T177" s="14">
+        <v>1.15610117E8</v>
+      </c>
+      <c r="X177" s="15">
+        <f t="shared" si="1"/>
+        <v>975</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2">
+        <v>45147.3919717824</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="F178" s="3">
+        <v>86.0</v>
+      </c>
+      <c r="G178" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H178" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I178" s="13">
+        <v>27.8</v>
+      </c>
+      <c r="T178" s="14">
+        <v>1.15610122E8</v>
+      </c>
+      <c r="X178" s="15">
+        <f t="shared" si="1"/>
+        <v>2390.8</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2">
+        <v>45147.39258770834</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="F179" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H179" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I179" s="13">
+        <v>1.2</v>
+      </c>
+      <c r="T179" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X179" s="15">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2">
+        <v>45147.39300671296</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="F180" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H180" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I180" s="13">
+        <v>1.25</v>
+      </c>
+      <c r="T180" s="14">
+        <v>1.15610116E8</v>
+      </c>
+      <c r="X180" s="15">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$Z$173"/>
+  <autoFilter ref="$A$1:$Z$180"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>